<commit_message>
Added deployment .py script
</commit_message>
<xml_diff>
--- a/capstone-results.xlsx
+++ b/capstone-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tungnguyen/Documents/repos/mec-capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B34353-7E06-ED4D-9142-CC7E34546FE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9666EF7-F05B-0240-8479-4DB3A86EEBD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="4" xr2:uid="{FCB33023-3F82-2347-A57C-137D11096206}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" activeTab="4" xr2:uid="{FCB33023-3F82-2347-A57C-137D11096206}"/>
   </bookViews>
   <sheets>
     <sheet name="Results_Round_1" sheetId="2" r:id="rId1"/>
@@ -683,6 +683,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -692,9 +695,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -702,47 +702,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1114,6 +1074,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>932246</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>180044</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F8C4D1C-9380-3E48-9158-5B134FE909B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7500362" y="6598478"/>
+          <a:ext cx="3858768" cy="2692436"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>932247</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>178741</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87061937-BF8B-D44F-908C-3D1E024279E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12377899" y="6598478"/>
+          <a:ext cx="3858768" cy="2691133"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2404,18 +2452,18 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="C5:L5">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>$O5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>$N5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:L18">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>$O6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>$N6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2444,20 +2492,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="51" t="s">
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="54"/>
     </row>
     <row r="3" spans="1:16" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
@@ -4256,18 +4304,18 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="C5:H5">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>$K5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>$J5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:H18">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>$K6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>$J6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5026,18 +5074,18 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="C5:H5">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>$K5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>$J5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:H18">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>$K6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>$J6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5049,8 +5097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B3709C-A7B4-8948-87D9-90DFF4277629}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="171" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I23" zoomScale="211" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5097,7 +5145,7 @@
       <c r="C4" s="41">
         <v>11</v>
       </c>
-      <c r="D4" s="54">
+      <c r="D4" s="51">
         <v>13.1</v>
       </c>
       <c r="F4" s="10" t="s">
@@ -5122,11 +5170,11 @@
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="7">
-        <f>MAX(C5:D5)</f>
+        <f t="shared" ref="F5:F18" si="0">MAX(C5:D5)</f>
         <v>0.78879999999999995</v>
       </c>
       <c r="G5" s="21">
-        <f>MIN(C5:D5)</f>
+        <f t="shared" ref="G5:G18" si="1">MIN(C5:D5)</f>
         <v>0.75770000000000004</v>
       </c>
     </row>
@@ -5145,11 +5193,11 @@
       </c>
       <c r="E6" s="24"/>
       <c r="F6" s="4">
-        <f>MAX(C6:D6)</f>
+        <f t="shared" si="0"/>
         <v>0.90429999999999999</v>
       </c>
       <c r="G6" s="22">
-        <f>MIN(C6:D6)</f>
+        <f t="shared" si="1"/>
         <v>0.88229999999999997</v>
       </c>
     </row>
@@ -5168,11 +5216,11 @@
       </c>
       <c r="E7" s="24"/>
       <c r="F7" s="4">
-        <f>MAX(C7:D7)</f>
+        <f t="shared" si="0"/>
         <v>0.77790000000000004</v>
       </c>
       <c r="G7" s="22">
-        <f>MIN(C7:D7)</f>
+        <f t="shared" si="1"/>
         <v>0.76749999999999996</v>
       </c>
     </row>
@@ -5191,11 +5239,11 @@
       </c>
       <c r="E8" s="24"/>
       <c r="F8" s="4">
-        <f>MAX(C8:D8)</f>
+        <f t="shared" si="0"/>
         <v>0.88819999999999999</v>
       </c>
       <c r="G8" s="22">
-        <f>MIN(C8:D8)</f>
+        <f t="shared" si="1"/>
         <v>0.86990000000000001</v>
       </c>
     </row>
@@ -5214,11 +5262,11 @@
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="4">
-        <f>MAX(C9:D9)</f>
+        <f t="shared" si="0"/>
         <v>0.85450000000000004</v>
       </c>
       <c r="G9" s="22">
-        <f>MIN(C9:D9)</f>
+        <f t="shared" si="1"/>
         <v>0.84340000000000004</v>
       </c>
     </row>
@@ -5237,11 +5285,11 @@
       </c>
       <c r="E10" s="24"/>
       <c r="F10" s="4">
-        <f>MAX(C10:D10)</f>
+        <f t="shared" si="0"/>
         <v>0.90680000000000005</v>
       </c>
       <c r="G10" s="22">
-        <f>MIN(C10:D10)</f>
+        <f t="shared" si="1"/>
         <v>0.88139999999999996</v>
       </c>
     </row>
@@ -5260,11 +5308,11 @@
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="4">
-        <f>MAX(C11:D11)</f>
+        <f t="shared" si="0"/>
         <v>0.77280000000000004</v>
       </c>
       <c r="G11" s="22">
-        <f>MIN(C11:D11)</f>
+        <f t="shared" si="1"/>
         <v>0.76880000000000004</v>
       </c>
     </row>
@@ -5283,11 +5331,11 @@
       </c>
       <c r="E12" s="24"/>
       <c r="F12" s="4">
-        <f>MAX(C12:D12)</f>
+        <f t="shared" si="0"/>
         <v>0.92279999999999995</v>
       </c>
       <c r="G12" s="22">
-        <f>MIN(C12:D12)</f>
+        <f t="shared" si="1"/>
         <v>0.88859999999999995</v>
       </c>
     </row>
@@ -5306,11 +5354,11 @@
       </c>
       <c r="E13" s="24"/>
       <c r="F13" s="4">
-        <f>MAX(C13:D13)</f>
+        <f t="shared" si="0"/>
         <v>0.65549999999999997</v>
       </c>
       <c r="G13" s="22">
-        <f>MIN(C13:D13)</f>
+        <f t="shared" si="1"/>
         <v>0.61939999999999995</v>
       </c>
     </row>
@@ -5329,11 +5377,11 @@
       </c>
       <c r="E14" s="24"/>
       <c r="F14" s="4">
-        <f>MAX(C14:D14)</f>
+        <f t="shared" si="0"/>
         <v>0.83199999999999996</v>
       </c>
       <c r="G14" s="22">
-        <f>MIN(C14:D14)</f>
+        <f t="shared" si="1"/>
         <v>0.82909999999999995</v>
       </c>
     </row>
@@ -5352,11 +5400,11 @@
       </c>
       <c r="E15" s="24"/>
       <c r="F15" s="4">
-        <f>MAX(C15:D15)</f>
+        <f t="shared" si="0"/>
         <v>0.72230000000000005</v>
       </c>
       <c r="G15" s="22">
-        <f>MIN(C15:D15)</f>
+        <f t="shared" si="1"/>
         <v>0.72130000000000005</v>
       </c>
     </row>
@@ -5375,11 +5423,11 @@
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="4">
-        <f>MAX(C16:D16)</f>
+        <f t="shared" si="0"/>
         <v>0.75949999999999995</v>
       </c>
       <c r="G16" s="22">
-        <f>MIN(C16:D16)</f>
+        <f t="shared" si="1"/>
         <v>0.75629999999999997</v>
       </c>
     </row>
@@ -5398,11 +5446,11 @@
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="4">
-        <f>MAX(C17:D17)</f>
+        <f t="shared" si="0"/>
         <v>0.73760000000000003</v>
       </c>
       <c r="G17" s="22">
-        <f>MIN(C17:D17)</f>
+        <f t="shared" si="1"/>
         <v>0.69169999999999998</v>
       </c>
     </row>
@@ -5421,11 +5469,11 @@
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="18">
-        <f>MAX(C18:D18)</f>
+        <f t="shared" si="0"/>
         <v>0.85829999999999995</v>
       </c>
       <c r="G18" s="23">
-        <f>MIN(C18:D18)</f>
+        <f t="shared" si="1"/>
         <v>0.84240000000000004</v>
       </c>
     </row>
@@ -5504,12 +5552,12 @@
     <mergeCell ref="N3:Q3"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:D5">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>$F5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D18">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>$F6</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>